<commit_message>
why does OT hate m
</commit_message>
<xml_diff>
--- a/opentable_03_18.xlsx
+++ b/opentable_03_18.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johntomczak/Documents/1Projects/Corona_DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1945F39C-9FAF-8446-A103-832722C0F29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1782BA-C173-774B-BE91-05CC0FB1AF0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -116,12 +116,6 @@
     <t>Minneapolis</t>
   </si>
   <si>
-    <t>Montr√©al</t>
-  </si>
-  <si>
-    <t>M√ºnchen</t>
-  </si>
-  <si>
     <t>Naples</t>
   </si>
   <si>
@@ -178,11 +172,17 @@
   <si>
     <t>Ciudad de Mexico</t>
   </si>
+  <si>
+    <t>Munchen</t>
+  </si>
+  <si>
+    <t>Montreal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1020,14 +1020,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1886,7 +1889,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2">
         <v>-0.08</v>
@@ -3596,7 +3599,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2">
         <v>0.16</v>
@@ -3691,7 +3694,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2">
         <v>0.08</v>
@@ -3786,7 +3789,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>-0.02</v>
@@ -3881,7 +3884,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>0.13</v>
@@ -3976,7 +3979,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>-0.09</v>
@@ -4166,7 +4169,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2">
         <v>-0.06</v>
@@ -4261,7 +4264,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2">
         <v>0.1</v>
@@ -4356,7 +4359,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2">
         <v>-0.04</v>
@@ -4451,7 +4454,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2">
         <v>0.1</v>
@@ -4546,7 +4549,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2">
         <v>0.01</v>
@@ -4641,7 +4644,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2">
         <v>7.0000000000000007E-2</v>
@@ -4736,7 +4739,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2">
         <v>-0.06</v>
@@ -4831,7 +4834,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2">
         <v>-0.01</v>
@@ -4926,7 +4929,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2">
         <v>-0.15</v>
@@ -5021,7 +5024,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2">
         <v>-0.09</v>
@@ -5116,7 +5119,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2">
         <v>-0.03</v>
@@ -5211,7 +5214,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2">
         <v>0.08</v>
@@ -5306,7 +5309,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="2">
         <v>7.0000000000000007E-2</v>
@@ -5401,7 +5404,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2">
         <v>-0.14000000000000001</v>
@@ -5496,7 +5499,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="2">
         <v>0.09</v>

</xml_diff>